<commit_message>
Finished most everything, some information is entered in the database to play around with. Currently working on a version that supports a webhosted database and stores files within dropbox. This will allow anyone in the company to access the inventory info and purchase orders sheets
</commit_message>
<xml_diff>
--- a/inventory_files/inventory_template.xlsx
+++ b/inventory_files/inventory_template.xlsx
@@ -1,24 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\napaf\Desktop\programming\adco_project\inventory_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E9F0E8-FF78-4078-B01B-925F03370795}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4365DC3-39CE-4B71-8438-D09423A5C257}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{4CE8CFAE-782F-4CC5-8497-1F069CB39A98}"/>
+    <workbookView xWindow="1360" yWindow="2840" windowWidth="14400" windowHeight="7360" firstSheet="12" activeTab="12" xr2:uid="{4CE8CFAE-782F-4CC5-8497-1F069CB39A98}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Materials" sheetId="1" r:id="rId1"/>
-    <sheet name="Bottles" sheetId="2" r:id="rId2"/>
-    <sheet name="Samples" sheetId="3" r:id="rId3"/>
-    <sheet name="Grain" sheetId="4" r:id="rId4"/>
-    <sheet name="Barrels" sheetId="5" r:id="rId5"/>
-    <sheet name="Purchase Orders" sheetId="6" r:id="rId6"/>
+    <sheet name="Production Log" sheetId="8" r:id="rId2"/>
+    <sheet name="In Progress" sheetId="9" r:id="rId3"/>
+    <sheet name="Bottles" sheetId="2" r:id="rId4"/>
+    <sheet name="Samples" sheetId="3" r:id="rId5"/>
+    <sheet name="Grain" sheetId="4" r:id="rId6"/>
+    <sheet name="Mash Log" sheetId="10" r:id="rId7"/>
+    <sheet name="Grain Log" sheetId="11" r:id="rId8"/>
+    <sheet name="Barrels" sheetId="5" r:id="rId9"/>
+    <sheet name="Emptied Barrels" sheetId="12" r:id="rId10"/>
+    <sheet name="Purchase Orders" sheetId="6" r:id="rId11"/>
+    <sheet name="Pending Purchase Orders" sheetId="7" r:id="rId12"/>
+    <sheet name="Employee Transactions" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
   <si>
     <t>Type</t>
   </si>
@@ -84,6 +91,42 @@
   </si>
   <si>
     <t>PO No.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Mash No</t>
+  </si>
+  <si>
+    <t>Grains</t>
+  </si>
+  <si>
+    <t>Arrival</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Order No</t>
+  </si>
+  <si>
+    <t>Barrel No</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>PG Leftover</t>
+  </si>
+  <si>
+    <t>Filled</t>
+  </si>
+  <si>
+    <t>Emptied</t>
+  </si>
+  <si>
+    <t>Employee</t>
   </si>
 </sst>
 </file>
@@ -514,7 +557,243 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672CB278-2B49-44C0-B3FB-BE071C65B7AD}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="9" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EA3A1C-4080-4A73-BB3F-5F44B2589A35}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="9" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46B4D6D-9F60-4D02-8E3F-AF12AC853681}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="9" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC348D4-A08F-4328-B812-C498CD9EA309}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="6" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10874057-1B90-4D43-B002-932D3C4428AA}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A47F8E3-59E0-4CC5-9167-76118E0D394C}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62CEC643-8252-4F1F-A4D8-A05244700679}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -552,7 +831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{348D4582-BEE7-404C-9667-94AF09CCB056}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -590,13 +869,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9640204-EFDE-4742-B861-69855D871BA5}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -628,13 +905,73 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894F7153-9B18-4373-A552-3DF4BBABF993}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694B1EA4-5F26-4B60-B959-2E5A0A1BF269}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AC9032D-F399-405A-81E7-B95C70DE8AEB}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -669,51 +1006,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EA3A1C-4080-4A73-BB3F-5F44B2589A35}">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="9" width="15.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>